<commit_message>
Fixing key times and samples for LSL
</commit_message>
<xml_diff>
--- a/common/sentences_s2.xlsx
+++ b/common/sentences_s2.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JARS\RST_psychopy\common\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="345" windowWidth="18675" windowHeight="11550"/>
+    <workbookView xWindow="360" yWindow="348" windowWidth="18672" windowHeight="11556"/>
   </bookViews>
   <sheets>
     <sheet name="sentences_s2" sheetId="1" r:id="rId1"/>
@@ -767,6 +772,7 @@
     <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
@@ -783,7 +789,6 @@
     <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
@@ -793,6 +798,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -841,7 +849,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -876,7 +884,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1087,411 +1095,413 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>80</v>
       </c>

</xml_diff>